<commit_message>
update xlsx and add videos
</commit_message>
<xml_diff>
--- a/Настройка_ПИД.xlsx
+++ b/Настройка_ПИД.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ITMO_2024_WORK\ITMO_Qt_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768F7A57-FBFB-48A8-B417-8B299F32820B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85951B54-E16F-489A-B116-C3FD10935007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -196,6 +196,106 @@
         </r>
       </text>
     </comment>
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{755741AF-EC76-46D1-A682-FC7B5C6C901A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Илья:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">Заменили плечо. Перевал через горизонт после </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>1530</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve"> (взлет и начинает переваливаться). Отрыв от земли в </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">1460.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Добавил оффсет +1 к ошибке (</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <u/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>к фильтру ни в коем случае</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>). Пока особой разницы не видно.
+Изменение throttle с 1470 до 1510 немного увеличила шанс перевала, но стало ровнее явно.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -255,7 +355,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,6 +438,15 @@
       <color indexed="81"/>
       <name val="Consolas"/>
       <family val="3"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
       <charset val="204"/>
     </font>
   </fonts>
@@ -674,7 +783,7 @@
   <dimension ref="A1:I312"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,14 +949,28 @@
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="A8" s="2">
+        <v>45390</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1.8</v>
+      </c>
+      <c r="C8" s="6">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1580</v>
+      </c>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1">
+        <v>1510</v>
+      </c>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" ht="21" x14ac:dyDescent="0.35">

</xml_diff>